<commit_message>
Class.forName changes in caller.java
</commit_message>
<xml_diff>
--- a/ExcelData/ExcelInput.xlsx
+++ b/ExcelData/ExcelInput.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinaygopinath/Documents/workspace/SeleniumMVNProject/ExcelData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinaygopinath/IdeaProjects/SeleniumFrameworkDemo/ExcelData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{503A7BE9-9FA2-2C4D-8BE3-B6F67574E523}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF8A6544-ACB5-624F-A8B0-59E045746F7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2380" yWindow="960" windowWidth="27640" windowHeight="15980" xr2:uid="{4AAF7CB0-C255-8C4E-84BF-A3EA88915242}"/>
+    <workbookView xWindow="1160" yWindow="960" windowWidth="27640" windowHeight="15980" xr2:uid="{4AAF7CB0-C255-8C4E-84BF-A3EA88915242}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Chapter1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,41 +35,46 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="8">
-  <si>
-    <t>demo test from Excel</t>
-  </si>
-  <si>
-    <t>demo test from Excel from different column</t>
-  </si>
-  <si>
-    <t>Excel String Data</t>
-  </si>
-  <si>
-    <t>Excel String Data1</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>3.2</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>SL No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Case Description </t>
+  </si>
+  <si>
+    <t>Test case Class Name</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>TestCase1</t>
+  </si>
+  <si>
+    <t>This test case is to test the input box</t>
+  </si>
+  <si>
+    <t>This test case is to test the drop down menu</t>
+  </si>
+  <si>
+    <t>TestCase2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -95,8 +100,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,33 +419,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4469489D-F7DD-2B4B-A0C5-97419C83FC6A}">
-  <dimension ref="B1:B7"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="38.1640625" collapsed="true"/>
+    <col min="2" max="2" width="40.5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.1640625" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="4">
-      <c r="C4" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>1</v>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added driver related if statements.
</commit_message>
<xml_diff>
--- a/ExcelData/ExcelInput.xlsx
+++ b/ExcelData/ExcelInput.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinaygopinath/IdeaProjects/SeleniumFrameworkDemo/ExcelData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF8A6544-ACB5-624F-A8B0-59E045746F7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B5DB43-30B4-894E-BE1F-D0D379B64F6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="960" windowWidth="27640" windowHeight="15980" xr2:uid="{4AAF7CB0-C255-8C4E-84BF-A3EA88915242}"/>
   </bookViews>
   <sheets>
-    <sheet name="Chapter1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Browser" sheetId="4" r:id="rId1"/>
+    <sheet name="Chapter1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>SL No</t>
   </si>
@@ -59,6 +60,12 @@
   </si>
   <si>
     <t>TestCase2</t>
+  </si>
+  <si>
+    <t>BrowserName</t>
+  </si>
+  <si>
+    <t>chrome</t>
   </si>
 </sst>
 </file>
@@ -418,10 +425,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3A7CEE3-59F2-B049-8B00-3BAF119210A1}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4469489D-F7DD-2B4B-A0C5-97419C83FC6A}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -474,7 +509,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDB5F849-1904-5840-B07F-20E3EC7C069D}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -486,7 +521,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32FB408A-D1EC-2C49-B41B-10F0D909BEA6}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
added Timestamp func and error handling
</commit_message>
<xml_diff>
--- a/ExcelData/ExcelInput.xlsx
+++ b/ExcelData/ExcelInput.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinaygopinath/IdeaProjects/SeleniumFrameworkDemo/ExcelData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B5DB43-30B4-894E-BE1F-D0D379B64F6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC2050A-3BD4-9348-AC7D-453B7974D409}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="960" windowWidth="27640" windowHeight="15980" xr2:uid="{4AAF7CB0-C255-8C4E-84BF-A3EA88915242}"/>
+    <workbookView xWindow="1160" yWindow="960" windowWidth="27640" windowHeight="15980" activeTab="1" xr2:uid="{4AAF7CB0-C255-8C4E-84BF-A3EA88915242}"/>
   </bookViews>
   <sheets>
     <sheet name="Browser" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>SL No</t>
   </si>
@@ -53,9 +53,6 @@
     <t>TestCase1</t>
   </si>
   <si>
-    <t>This test case is to test the input box</t>
-  </si>
-  <si>
     <t>This test case is to test the drop down menu</t>
   </si>
   <si>
@@ -66,12 +63,40 @@
   </si>
   <si>
     <t>chrome</t>
+  </si>
+  <si>
+    <t>TimeStamp</t>
+  </si>
+  <si>
+    <t>Test Data</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>This test case is to test the txt field</t>
+  </si>
+  <si>
+    <t>2020-06-10 16:35:33.964</t>
+  </si>
+  <si>
+    <t>2020-06-10 16:35:41.098</t>
+  </si>
+  <si>
+    <t>Test Message from Excel</t>
+  </si>
+  <si>
+    <t>2020-06-10 16:38:59.734</t>
+  </si>
+  <si>
+    <t>2020-06-10 16:39:06.907</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -428,23 +453,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3A7CEE3-59F2-B049-8B00-3BAF119210A1}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -454,20 +479,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4469489D-F7DD-2B4B-A0C5-97419C83FC6A}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="40.5" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.1640625" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="40.5" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.1640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="22.33203125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -480,27 +507,48 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>